<commit_message>
added supportive excel db and created another two tables with wrong data eh
</commit_message>
<xml_diff>
--- a/statystyki.xlsx
+++ b/statystyki.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41240" yWindow="5240" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="440" windowWidth="26820" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <f>(45-E2)/((D2-C2+1)*F2)</f>
+        <f t="shared" ref="G2:G16" si="0">(45-E2)/((D2-C2+1)*F2)</f>
         <v>18.25</v>
       </c>
     </row>
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <f>(45-E3)/((D3-C3+1)*F3)</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
     </row>
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <f>(45-E4)/((D4-C4+1)*F4)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -557,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <f>(45-E5)/((D5-C5+1)*F5)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <f>(45-E6)/((D6-C6+1)*F6)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
     </row>
@@ -605,7 +605,7 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <f>(45-E7)/((D7-C7+1)*F7)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <f>(45-E8)/((D8-C8+1)*F8)</f>
+        <f t="shared" si="0"/>
         <v>12.25</v>
       </c>
     </row>
@@ -653,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <f>(45-E9)/((D9-C9+1)*F9)</f>
+        <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
     </row>
@@ -677,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <f>(45-E10)/((D10-C10+1)*F10)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <f>(45-E11)/((D11-C11+1)*F11)</f>
+        <f t="shared" si="0"/>
         <v>7.666666666666667</v>
       </c>
     </row>
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="G12">
-        <f>(45-E12)/((D12-C12+1)*F12)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
@@ -749,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <f>(45-E13)/((D13-C13+1)*F13)</f>
+        <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
     </row>
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="G14">
-        <f>(45-E14)/((D14-C14+1)*F14)</f>
+        <f t="shared" si="0"/>
         <v>10.375</v>
       </c>
     </row>
@@ -797,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <f>(45-E15)/((D15-C15+1)*F15)</f>
+        <f t="shared" si="0"/>
         <v>5.833333333333333</v>
       </c>
     </row>
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
       <c r="G16">
-        <f>(45-E16)/((D16-C16+1)*F16)</f>
+        <f t="shared" si="0"/>
         <v>2.9166666666666665</v>
       </c>
     </row>

</xml_diff>